<commit_message>
Atualização de novos documentos
</commit_message>
<xml_diff>
--- a/Documentos/CADASTRO.xlsx
+++ b/Documentos/CADASTRO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332BDC8F-3A5E-4AC1-A982-57DA505E71E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5DA89C-70BE-43B6-85A7-02D083DAADA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D97F085D-39BF-40A8-913E-D715D9E5FECC}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="194">
   <si>
     <t>CONT_ID</t>
   </si>
@@ -622,6 +622,9 @@
   </si>
   <si>
     <t>detail_epro,config_epro</t>
+  </si>
+  <si>
+    <t>ENEL</t>
   </si>
 </sst>
 </file>
@@ -2818,10 +2821,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1104F42-6122-4AF9-A63B-0A323A430B6D}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2948,11 +2951,11 @@
       </c>
       <c r="Q2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -3000,11 +3003,11 @@
       </c>
       <c r="Q3" s="6">
         <f t="shared" ref="Q3:R16" ca="1" si="0">TODAY()</f>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -3052,11 +3055,11 @@
       </c>
       <c r="Q4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -3104,11 +3107,11 @@
       </c>
       <c r="Q5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -3156,11 +3159,11 @@
       </c>
       <c r="Q6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -3208,11 +3211,11 @@
       </c>
       <c r="Q7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -3260,11 +3263,11 @@
       </c>
       <c r="Q8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -3312,11 +3315,11 @@
       </c>
       <c r="Q9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3364,11 +3367,11 @@
       </c>
       <c r="Q10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -3416,11 +3419,11 @@
       </c>
       <c r="Q11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -3468,11 +3471,11 @@
       </c>
       <c r="Q12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -3520,11 +3523,11 @@
       </c>
       <c r="Q13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -3572,11 +3575,11 @@
       </c>
       <c r="Q14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -3624,11 +3627,11 @@
       </c>
       <c r="Q15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -3676,26 +3679,43 @@
       </c>
       <c r="Q16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
+        <v>45469</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45468</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="F18" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="2" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Acordos e Pagamentos Actyon mapeados
</commit_message>
<xml_diff>
--- a/Documentos/CADASTRO.xlsx
+++ b/Documentos/CADASTRO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5DA89C-70BE-43B6-85A7-02D083DAADA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47703B1A-7E91-4A46-B51B-4FD94A7FFCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D97F085D-39BF-40A8-913E-D715D9E5FECC}"/>
   </bookViews>
@@ -2824,7 +2824,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2951,11 +2951,11 @@
       </c>
       <c r="Q2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -3003,11 +3003,11 @@
       </c>
       <c r="Q3" s="6">
         <f t="shared" ref="Q3:R16" ca="1" si="0">TODAY()</f>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -3055,11 +3055,11 @@
       </c>
       <c r="Q4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -3107,11 +3107,11 @@
       </c>
       <c r="Q5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -3159,11 +3159,11 @@
       </c>
       <c r="Q6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -3211,11 +3211,11 @@
       </c>
       <c r="Q7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -3263,11 +3263,11 @@
       </c>
       <c r="Q8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -3315,11 +3315,11 @@
       </c>
       <c r="Q9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3367,11 +3367,11 @@
       </c>
       <c r="Q10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -3419,11 +3419,11 @@
       </c>
       <c r="Q11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -3471,11 +3471,11 @@
       </c>
       <c r="Q12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -3523,11 +3523,11 @@
       </c>
       <c r="Q13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -3575,11 +3575,11 @@
       </c>
       <c r="Q14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R14" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -3627,11 +3627,11 @@
       </c>
       <c r="Q15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -3679,11 +3679,11 @@
       </c>
       <c r="Q16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
       <c r="R16" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45469</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>